<commit_message>
Cambios de impresion en guia
</commit_message>
<xml_diff>
--- a/output/JAL/importar sodimac.xlsx
+++ b/output/JAL/importar sodimac.xlsx
@@ -676,7 +676,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB2"/>
+  <dimension ref="A1:AB3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B3"/>
@@ -858,12 +858,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>16255167</t>
+          <t>16479386</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>16255167</t>
+          <t>16479386</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -888,12 +888,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>20250506</t>
+          <t>20250729</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>20250509</t>
+          <t>20250801</t>
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
@@ -912,7 +912,7 @@
         </is>
       </c>
       <c r="T2" t="n">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr"/>
@@ -921,7 +921,77 @@
       <c r="AA2" t="inlineStr"/>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>1588</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>16479386</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>16479386</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>96792430-K</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>SODIMAC S.A.</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>SODIMAC</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>CD 221</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>20250729</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>20250801</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>7641117</t>
+        </is>
+      </c>
+      <c r="T3" t="n">
+        <v>24</v>
+      </c>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>1588</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add: tottus and sodimac
</commit_message>
<xml_diff>
--- a/output/JAL/importar sodimac.xlsx
+++ b/output/JAL/importar sodimac.xlsx
@@ -68,7 +68,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -77,7 +77,6 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,10 +675,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB3"/>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -706,11 +705,11 @@
     <col width="17.5703125" bestFit="1" customWidth="1" style="3" min="20" max="20"/>
     <col hidden="1" width="13.7109375" customWidth="1" style="3" min="21" max="21"/>
     <col hidden="1" width="12.85546875" customWidth="1" style="2" min="22" max="22"/>
-    <col width="8.28515625" bestFit="1" customWidth="1" style="8" min="23" max="23"/>
-    <col width="11.85546875" bestFit="1" customWidth="1" style="8" min="24" max="24"/>
-    <col width="15" bestFit="1" customWidth="1" style="8" min="25" max="25"/>
-    <col width="10.7109375" bestFit="1" customWidth="1" style="8" min="26" max="26"/>
-    <col width="11.28515625" bestFit="1" customWidth="1" style="8" min="27" max="27"/>
+    <col width="8.28515625" bestFit="1" customWidth="1" min="23" max="23"/>
+    <col width="11.85546875" bestFit="1" customWidth="1" min="24" max="24"/>
+    <col width="15" bestFit="1" customWidth="1" min="25" max="25"/>
+    <col width="10.7109375" bestFit="1" customWidth="1" min="26" max="26"/>
+    <col width="11.28515625" bestFit="1" customWidth="1" min="27" max="27"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -858,12 +857,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>16479386</t>
+          <t>16522831</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>16479386</t>
+          <t>16522831</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -888,12 +887,12 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>20250729</t>
+          <t>20250814</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>20250801</t>
+          <t>20250828</t>
         </is>
       </c>
       <c r="I2" t="inlineStr"/>
@@ -912,7 +911,7 @@
         </is>
       </c>
       <c r="T2" t="n">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr"/>
@@ -921,77 +920,7 @@
       <c r="AA2" t="inlineStr"/>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>1588</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>16479386</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>16479386</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>96792430-K</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>SODIMAC S.A.</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>SODIMAC</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>CD 221</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>20250729</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>20250801</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
-      <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
-      <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>7641117</t>
-        </is>
-      </c>
-      <c r="T3" t="n">
-        <v>24</v>
-      </c>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
-      <c r="Z3" t="inlineStr"/>
-      <c r="AA3" t="inlineStr"/>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>1588</t>
+          <t>1612</t>
         </is>
       </c>
     </row>

</xml_diff>